<commit_message>
20171121 2344 update schedule
</commit_message>
<xml_diff>
--- a/notes/2017_2nd_half_schedule_template.xlsx
+++ b/notes/2017_2nd_half_schedule_template.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\yfhosanna\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\workspace\ridiculands-reference\master\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="11916"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="11910"/>
   </bookViews>
   <sheets>
     <sheet name="繁" sheetId="1" r:id="rId1"/>
     <sheet name="簡" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="71">
   <si>
     <t>領詩</t>
   </si>
@@ -99,12 +99,6 @@
     <t>生命查經 19</t>
   </si>
   <si>
-    <t>外出報佳音</t>
-  </si>
-  <si>
-    <t>下午帶親友去聖誔佈道會</t>
-  </si>
-  <si>
     <t>生命查經 20</t>
   </si>
   <si>
@@ -240,13 +234,16 @@
     <t>恩典组</t>
   </si>
   <si>
-    <t>aaa</t>
+    <t>大組生命查經（太 2:1-12）</t>
+  </si>
+  <si>
+    <t>醫院報佳音（2pm-5pm）</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -289,7 +286,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -604,19 +601,19 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="47.77734375" style="2" customWidth="1"/>
-    <col min="3" max="8" width="11.109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="72.21875" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="17.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="47.7109375" style="2" customWidth="1"/>
+    <col min="3" max="8" width="11.140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="72.28515625" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
         <v>42910</v>
       </c>
@@ -627,7 +624,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>1</v>
@@ -636,14 +633,14 @@
         <v>2</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I1" s="2" t="str">
         <f>_xlfn.CONCAT(B1, "　（", C1, "︰", D1, "，", E1, "︰", F1, "，", G1, "︰", H1, "）")</f>
         <v>生命查經 9　（領詩︰Jabez，小食︰，司事︰Issac）</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>42917</v>
       </c>
@@ -660,7 +657,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>42924</v>
       </c>
@@ -671,22 +668,22 @@
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>42931</v>
       </c>
@@ -697,7 +694,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>1</v>
@@ -706,10 +703,10 @@
         <v>2</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>42938</v>
       </c>
@@ -720,7 +717,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>1</v>
@@ -729,10 +726,10 @@
         <v>2</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>42945</v>
       </c>
@@ -743,7 +740,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>1</v>
@@ -752,10 +749,10 @@
         <v>2</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>42952</v>
       </c>
@@ -772,7 +769,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>42959</v>
       </c>
@@ -783,33 +780,33 @@
         <v>0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>2</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>42966</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>1</v>
@@ -818,10 +815,10 @@
         <v>2</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>42973</v>
       </c>
@@ -838,33 +835,33 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>42980</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>2</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>42987</v>
       </c>
@@ -875,7 +872,7 @@
         <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>1</v>
@@ -884,10 +881,10 @@
         <v>2</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>42994</v>
       </c>
@@ -904,7 +901,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>43001</v>
       </c>
@@ -921,7 +918,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>43008</v>
       </c>
@@ -932,7 +929,7 @@
         <v>0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>1</v>
@@ -941,10 +938,10 @@
         <v>2</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>43015</v>
       </c>
@@ -955,22 +952,22 @@
         <v>0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>2</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43022</v>
       </c>
@@ -987,7 +984,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>43029</v>
       </c>
@@ -998,7 +995,7 @@
         <v>0</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>1</v>
@@ -1007,10 +1004,10 @@
         <v>2</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>43036</v>
       </c>
@@ -1027,7 +1024,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>43043</v>
       </c>
@@ -1038,22 +1035,22 @@
         <v>0</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>2</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>43050</v>
       </c>
@@ -1064,7 +1061,7 @@
         <v>0</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>1</v>
@@ -1073,10 +1070,10 @@
         <v>2</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>43057</v>
       </c>
@@ -1087,7 +1084,7 @@
         <v>0</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>1</v>
@@ -1096,10 +1093,10 @@
         <v>2</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>43064</v>
       </c>
@@ -1110,7 +1107,7 @@
         <v>0</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>1</v>
@@ -1119,10 +1116,10 @@
         <v>2</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>43071</v>
       </c>
@@ -1139,7 +1136,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>43078</v>
       </c>
@@ -1150,44 +1147,54 @@
         <v>0</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>2</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>43085</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="D26" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="E26" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H26" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I26" s="2" t="str">
+        <f>CONCATENATE(IF(AND(ISBLANK(D26)=FALSE, ISBLANK(F26)=FALSE, ISBLANK(H26)=FALSE),"（",""), IF(ISBLANK(D26)=FALSE, CONCATENATE(C26, "︰", D26), ""), IF(ISBLANK(F26)=FALSE, CONCATENATE("，", E26, "︰", F26), ""), IF(ISBLANK(H26)=FALSE, CONCATENATE("，", G26, "︰", H26), ""), IF(AND(ISBLANK(D26)=FALSE, ISBLANK(F26)=FALSE, ISBLANK(H26)=FALSE),"）",""))</f>
+        <v>領詩︰Manna，司事︰Jabez</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>43092</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>0</v>
@@ -1198,22 +1205,23 @@
       <c r="G27" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I27" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I27" s="2" t="str">
+        <f>CONCATENATE(IF(AND(ISBLANK(D27)=FALSE, ISBLANK(F27)=FALSE, ISBLANK(H27)=FALSE),"（",""), IF(ISBLANK(D27)=FALSE, CONCATENATE(C27, "︰", D27), ""), IF(ISBLANK(F27)=FALSE, CONCATENATE("，", E27, "︰", F27), ""), IF(ISBLANK(H27)=FALSE, CONCATENATE("，", G27, "︰", H27), ""), IF(AND(ISBLANK(D27)=FALSE, ISBLANK(F27)=FALSE, ISBLANK(H27)=FALSE),"）",""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>43099</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>1</v>
@@ -1222,37 +1230,37 @@
         <v>2</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I28" s="2" t="str">
         <f>_xlfn.CONCAT(IF(ISBLANK(D28)=FALSE, _xlfn.CONCAT(C28, "︰", D28), ""), IF(ISBLANK(F28)=FALSE, _xlfn.CONCAT("，", E28, "︰", F28), ""), IF(ISBLANK(H28)=FALSE, _xlfn.CONCAT("，", G28, "︰", H28), ""))</f>
         <v>領詩︰Manna，司事︰Jabez</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>43106</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D29" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H29" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="I29" s="2" t="str">
         <f>_xlfn.CONCAT(IF(AND(ISBLANK(D29)=FALSE, ISBLANK(F29)=FALSE, ISBLANK(H29)=FALSE),"（",""), IF(ISBLANK(D29)=FALSE, _xlfn.CONCAT(C29, "︰", D29), ""), IF(ISBLANK(F29)=FALSE, _xlfn.CONCAT("，", E29, "︰", F29), ""), IF(ISBLANK(H29)=FALSE, _xlfn.CONCAT("，", G29, "︰", H29), ""), IF(AND(ISBLANK(D29)=FALSE, ISBLANK(F29)=FALSE, ISBLANK(H29)=FALSE),"）",""))</f>
@@ -1273,27 +1281,27 @@
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="47.77734375" style="2" customWidth="1"/>
-    <col min="3" max="8" width="11.109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="72.21875" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="17.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="47.7109375" style="2" customWidth="1"/>
+    <col min="3" max="8" width="11.140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="72.28515625" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
         <v>42910</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>1</v>
@@ -1302,15 +1310,15 @@
         <v>2</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>42917</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>3</v>
@@ -1322,44 +1330,44 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>42924</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>42931</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>1</v>
@@ -1368,21 +1376,21 @@
         <v>2</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>42938</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>1</v>
@@ -1391,21 +1399,21 @@
         <v>2</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>42945</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>1</v>
@@ -1414,15 +1422,15 @@
         <v>2</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>42952</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>3</v>
@@ -1434,44 +1442,44 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>42959</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>2</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>42966</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>1</v>
@@ -1480,15 +1488,15 @@
         <v>2</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>42973</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>3</v>
@@ -1500,44 +1508,44 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>42980</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>2</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>42987</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>1</v>
@@ -1546,15 +1554,15 @@
         <v>2</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>42994</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>3</v>
@@ -1566,12 +1574,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>43001</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>3</v>
@@ -1583,18 +1591,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>43008</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>1</v>
@@ -1603,41 +1611,41 @@
         <v>2</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>43015</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>2</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43022</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>3</v>
@@ -1649,18 +1657,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>43029</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>1</v>
@@ -1669,15 +1677,15 @@
         <v>2</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>43036</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>3</v>
@@ -1689,44 +1697,44 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>43043</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>2</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>43050</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>1</v>
@@ -1735,21 +1743,21 @@
         <v>2</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>43057</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>1</v>
@@ -1758,21 +1766,21 @@
         <v>2</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>43064</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>1</v>
@@ -1781,15 +1789,15 @@
         <v>2</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>43071</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>3</v>
@@ -1801,38 +1809,38 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>43078</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>2</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>43085</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>3</v>
@@ -1844,12 +1852,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>43092</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>3</v>
@@ -1861,18 +1869,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>43099</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>1</v>
@@ -1881,33 +1889,33 @@
         <v>2</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>43106</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D29" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H29" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>